<commit_message>
Updates to tracker, added MusicVAE folder
</commit_message>
<xml_diff>
--- a/Magenta_2_JazzBerryJam_Feature_Tracker.xlsx
+++ b/Magenta_2_JazzBerryJam_Feature_Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dataninjas-my.sharepoint.com/personal/clayton_e_tillman_dataninjas_onmicrosoft_com/Documents/Julia/JuliaLang/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Repos\JazzBerryJam\JazzberryJam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{808A809D-6C7F-49E3-B356-B2232C797753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{144D3161-C08B-4F5F-BED9-D52AA39065AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569EC684-67CD-4ABD-9EEB-475334A2003B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35350BD0-46B4-4F88-8FA8-515D9F08DFF9}"/>
+    <workbookView xWindow="-270" yWindow="-270" windowWidth="29100" windowHeight="14940" xr2:uid="{35350BD0-46B4-4F88-8FA8-515D9F08DFF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Magenta &gt; JBJ" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Julia counterpart</t>
   </si>
@@ -91,9 +91,6 @@
     <t xml:space="preserve">ninjadatum; </t>
   </si>
   <si>
-    <t>not feature complete, could pick up one of the items on the roadmap</t>
-  </si>
-  <si>
     <t>JuliaMusic/MusicProcessing.jl</t>
   </si>
   <si>
@@ -101,6 +98,30 @@
   </si>
   <si>
     <t>started 2021/07/30</t>
+  </si>
+  <si>
+    <t>not feature complete, could pick up one of the items on the roadmap; inspired by librosa (https://github.com/librosa/librosa)</t>
+  </si>
+  <si>
+    <t>machine learning model that lets us create palettes for blending and exploring musical scores</t>
+  </si>
+  <si>
+    <t>Neural Synthesizer</t>
+  </si>
+  <si>
+    <t>started 2021/07/30; could go on top of MPlay.jl (https://github.com/JuliaMusic/Mplay.jl) maybe</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>Mplay.jl</t>
+  </si>
+  <si>
+    <t>full functional MIDI player written in pure Julia</t>
+  </si>
+  <si>
+    <t>JazzberryJam/MusicVAE.jl</t>
   </si>
 </sst>
 </file>
@@ -485,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F52B361-E556-4B78-A0F4-69BCABFA2FEA}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +568,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,10 +582,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -574,6 +595,18 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -584,19 +617,17 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -610,27 +641,48 @@
     <hyperlink ref="A6" r:id="rId2" display="https://g.co/magenta/music-vae" xr:uid="{13193F09-60F7-4958-908F-94603419749F}"/>
     <hyperlink ref="A7" r:id="rId3" display="https://magenta.tensorflow.org/performance-rnn" xr:uid="{A06C6A44-B0C5-4D22-873B-87D4D8B8BB4F}"/>
     <hyperlink ref="A8" r:id="rId4" display="https://magenta.tensorflow.org/nsynth" xr:uid="{DD35D51F-0598-49F7-8779-703BB782C42D}"/>
-    <hyperlink ref="A9" r:id="rId5" display="https://g.co/magenta/music-vae" xr:uid="{096E1D74-196A-4D9A-970D-447F5AA2EE71}"/>
-    <hyperlink ref="A10" r:id="rId6" display="https://magenta.tensorflow.org/onsets-frames" xr:uid="{8CBC7B81-96F7-4DBB-930C-5D952BD9AD48}"/>
-    <hyperlink ref="A11" r:id="rId7" display="http://arxiv.org/abs/1711.05772" xr:uid="{EB5B32F5-007A-465C-A645-BF4B2B9240FF}"/>
-    <hyperlink ref="A3" r:id="rId8" display="https://magenta.tensorflow.org/ddsp" xr:uid="{E9A4A4A2-A6B3-4547-83A3-724B1880A9F1}"/>
-    <hyperlink ref="A4" r:id="rId9" display="https://magenta.tensorflow.org/music-transformer" xr:uid="{E92B39FA-7552-4571-A99C-2B07E755EDAA}"/>
-    <hyperlink ref="C4" r:id="rId10" display="https://github.com/JuliaMusic/MusicProcessing.jl" xr:uid="{3E5B7285-C46B-4496-BFFE-65BA12801FE1}"/>
-    <hyperlink ref="C5" r:id="rId11" tooltip="GANSynth.jl" display="https://github.com/claytonEtillman/JazzberryJam/tree/main/GANSynth.jl" xr:uid="{EEBB7EE3-88AA-47BF-80B6-341162EAF656}"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://magenta.tensorflow.org/onsets-frames" xr:uid="{8CBC7B81-96F7-4DBB-930C-5D952BD9AD48}"/>
+    <hyperlink ref="A10" r:id="rId6" display="http://arxiv.org/abs/1711.05772" xr:uid="{EB5B32F5-007A-465C-A645-BF4B2B9240FF}"/>
+    <hyperlink ref="A3" r:id="rId7" display="https://magenta.tensorflow.org/ddsp" xr:uid="{E9A4A4A2-A6B3-4547-83A3-724B1880A9F1}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://magenta.tensorflow.org/music-transformer" xr:uid="{E92B39FA-7552-4571-A99C-2B07E755EDAA}"/>
+    <hyperlink ref="C4" r:id="rId9" display="https://github.com/JuliaMusic/MusicProcessing.jl" xr:uid="{3E5B7285-C46B-4496-BFFE-65BA12801FE1}"/>
+    <hyperlink ref="C5" r:id="rId10" tooltip="GANSynth.jl" display="https://github.com/claytonEtillman/JazzberryJam/tree/main/GANSynth.jl" xr:uid="{EEBB7EE3-88AA-47BF-80B6-341162EAF656}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCA1EBA-15A5-4289-B422-4C28828972D6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://github.com/JuliaMusic/Mplay.jl" xr:uid="{719F77A1-E827-4C05-9AB7-285C54F11907}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>